<commit_message>
Tested and working with 16x16 character graphics
</commit_message>
<xml_diff>
--- a/Resources/Stack diagrams.xlsx
+++ b/Resources/Stack diagrams.xlsx
@@ -331,13 +331,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1008,84 +1008,84 @@
       <c r="BL7" s="13"/>
     </row>
     <row r="8" spans="1:64" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="F8" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="K8" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="L8" s="14"/>
-      <c r="M8" s="14"/>
-      <c r="N8" s="14"/>
-      <c r="P8" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q8" s="14"/>
-      <c r="R8" s="14"/>
-      <c r="S8" s="14"/>
-      <c r="U8" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="V8" s="14"/>
-      <c r="W8" s="14"/>
-      <c r="X8" s="14"/>
-      <c r="Z8" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="AA8" s="14"/>
-      <c r="AB8" s="14"/>
-      <c r="AC8" s="14"/>
-      <c r="AE8" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="AF8" s="14"/>
-      <c r="AG8" s="14"/>
-      <c r="AH8" s="14"/>
-      <c r="AJ8" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="AK8" s="14"/>
-      <c r="AL8" s="14"/>
-      <c r="AM8" s="14"/>
-      <c r="AO8" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="AP8" s="14"/>
-      <c r="AQ8" s="14"/>
-      <c r="AR8" s="14"/>
-      <c r="AT8" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="AU8" s="14"/>
-      <c r="AV8" s="14"/>
-      <c r="AW8" s="14"/>
-      <c r="AY8" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="AZ8" s="14"/>
-      <c r="BA8" s="14"/>
-      <c r="BB8" s="14"/>
-      <c r="BD8" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="BE8" s="14"/>
-      <c r="BF8" s="14"/>
-      <c r="BG8" s="14"/>
-      <c r="BI8" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="BJ8" s="14"/>
-      <c r="BK8" s="14"/>
-      <c r="BL8" s="14"/>
+      <c r="A8" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="F8" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+      <c r="K8" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="L8" s="16"/>
+      <c r="M8" s="16"/>
+      <c r="N8" s="16"/>
+      <c r="P8" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q8" s="16"/>
+      <c r="R8" s="16"/>
+      <c r="S8" s="16"/>
+      <c r="U8" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="V8" s="16"/>
+      <c r="W8" s="16"/>
+      <c r="X8" s="16"/>
+      <c r="Z8" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA8" s="16"/>
+      <c r="AB8" s="16"/>
+      <c r="AC8" s="16"/>
+      <c r="AE8" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="AF8" s="16"/>
+      <c r="AG8" s="16"/>
+      <c r="AH8" s="16"/>
+      <c r="AJ8" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="AK8" s="16"/>
+      <c r="AL8" s="16"/>
+      <c r="AM8" s="16"/>
+      <c r="AO8" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="AP8" s="16"/>
+      <c r="AQ8" s="16"/>
+      <c r="AR8" s="16"/>
+      <c r="AT8" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="AU8" s="16"/>
+      <c r="AV8" s="16"/>
+      <c r="AW8" s="16"/>
+      <c r="AY8" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="AZ8" s="16"/>
+      <c r="BA8" s="16"/>
+      <c r="BB8" s="16"/>
+      <c r="BD8" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="BE8" s="16"/>
+      <c r="BF8" s="16"/>
+      <c r="BG8" s="16"/>
+      <c r="BI8" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="BJ8" s="16"/>
+      <c r="BK8" s="16"/>
+      <c r="BL8" s="16"/>
     </row>
     <row r="9" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -1693,96 +1693,96 @@
       </c>
     </row>
     <row r="16" spans="1:64" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="14" t="s">
+      <c r="A16" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="F16" s="14" t="str">
+      <c r="B16" s="16"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="F16" s="16" t="str">
         <f>A16</f>
         <v>Subroutine stack</v>
       </c>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-      <c r="K16" s="14" t="str">
+      <c r="G16" s="16"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="16"/>
+      <c r="K16" s="16" t="str">
         <f>F16</f>
         <v>Subroutine stack</v>
       </c>
-      <c r="L16" s="14"/>
-      <c r="M16" s="14"/>
-      <c r="N16" s="14"/>
-      <c r="P16" s="14" t="str">
+      <c r="L16" s="16"/>
+      <c r="M16" s="16"/>
+      <c r="N16" s="16"/>
+      <c r="P16" s="16" t="str">
         <f>K16</f>
         <v>Subroutine stack</v>
       </c>
-      <c r="Q16" s="14"/>
-      <c r="R16" s="14"/>
-      <c r="S16" s="14"/>
-      <c r="U16" s="14" t="str">
+      <c r="Q16" s="16"/>
+      <c r="R16" s="16"/>
+      <c r="S16" s="16"/>
+      <c r="U16" s="16" t="str">
         <f>P16</f>
         <v>Subroutine stack</v>
       </c>
-      <c r="V16" s="14"/>
-      <c r="W16" s="14"/>
-      <c r="X16" s="14"/>
-      <c r="Z16" s="14" t="str">
+      <c r="V16" s="16"/>
+      <c r="W16" s="16"/>
+      <c r="X16" s="16"/>
+      <c r="Z16" s="16" t="str">
         <f>U16</f>
         <v>Subroutine stack</v>
       </c>
-      <c r="AA16" s="14"/>
-      <c r="AB16" s="14"/>
-      <c r="AC16" s="14"/>
-      <c r="AE16" s="14" t="str">
+      <c r="AA16" s="16"/>
+      <c r="AB16" s="16"/>
+      <c r="AC16" s="16"/>
+      <c r="AE16" s="16" t="str">
         <f>Z16</f>
         <v>Subroutine stack</v>
       </c>
-      <c r="AF16" s="14"/>
-      <c r="AG16" s="14"/>
-      <c r="AH16" s="14"/>
-      <c r="AJ16" s="14" t="str">
+      <c r="AF16" s="16"/>
+      <c r="AG16" s="16"/>
+      <c r="AH16" s="16"/>
+      <c r="AJ16" s="16" t="str">
         <f>AE16</f>
         <v>Subroutine stack</v>
       </c>
-      <c r="AK16" s="14"/>
-      <c r="AL16" s="14"/>
-      <c r="AM16" s="14"/>
-      <c r="AO16" s="14" t="str">
+      <c r="AK16" s="16"/>
+      <c r="AL16" s="16"/>
+      <c r="AM16" s="16"/>
+      <c r="AO16" s="16" t="str">
         <f>AJ16</f>
         <v>Subroutine stack</v>
       </c>
-      <c r="AP16" s="14"/>
-      <c r="AQ16" s="14"/>
-      <c r="AR16" s="14"/>
-      <c r="AT16" s="14" t="str">
+      <c r="AP16" s="16"/>
+      <c r="AQ16" s="16"/>
+      <c r="AR16" s="16"/>
+      <c r="AT16" s="16" t="str">
         <f>AO16</f>
         <v>Subroutine stack</v>
       </c>
-      <c r="AU16" s="14"/>
-      <c r="AV16" s="14"/>
-      <c r="AW16" s="14"/>
-      <c r="AY16" s="14">
+      <c r="AU16" s="16"/>
+      <c r="AV16" s="16"/>
+      <c r="AW16" s="16"/>
+      <c r="AY16" s="16">
         <f>BD16</f>
         <v>0</v>
       </c>
-      <c r="AZ16" s="14"/>
-      <c r="BA16" s="14"/>
-      <c r="BB16" s="14"/>
-      <c r="BD16" s="14">
+      <c r="AZ16" s="16"/>
+      <c r="BA16" s="16"/>
+      <c r="BB16" s="16"/>
+      <c r="BD16" s="16">
         <f>AU16</f>
         <v>0</v>
       </c>
-      <c r="BE16" s="14"/>
-      <c r="BF16" s="14"/>
-      <c r="BG16" s="14"/>
-      <c r="BI16" s="14">
+      <c r="BE16" s="16"/>
+      <c r="BF16" s="16"/>
+      <c r="BG16" s="16"/>
+      <c r="BI16" s="16">
         <f>BA16</f>
         <v>0</v>
       </c>
-      <c r="BJ16" s="14"/>
-      <c r="BK16" s="14"/>
-      <c r="BL16" s="14"/>
+      <c r="BJ16" s="16"/>
+      <c r="BK16" s="16"/>
+      <c r="BL16" s="16"/>
     </row>
     <row r="17" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
@@ -2589,96 +2589,96 @@
       </c>
     </row>
     <row r="26" spans="1:64" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="14" t="s">
+      <c r="A26" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B26" s="14"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="14"/>
-      <c r="F26" s="14" t="str">
+      <c r="B26" s="16"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="16"/>
+      <c r="F26" s="16" t="str">
         <f>A26</f>
         <v>Return stack</v>
       </c>
-      <c r="G26" s="14"/>
-      <c r="H26" s="14"/>
-      <c r="I26" s="14"/>
-      <c r="K26" s="14" t="str">
+      <c r="G26" s="16"/>
+      <c r="H26" s="16"/>
+      <c r="I26" s="16"/>
+      <c r="K26" s="16" t="str">
         <f>F26</f>
         <v>Return stack</v>
       </c>
-      <c r="L26" s="14"/>
-      <c r="M26" s="14"/>
-      <c r="N26" s="14"/>
-      <c r="P26" s="14" t="str">
+      <c r="L26" s="16"/>
+      <c r="M26" s="16"/>
+      <c r="N26" s="16"/>
+      <c r="P26" s="16" t="str">
         <f>K26</f>
         <v>Return stack</v>
       </c>
-      <c r="Q26" s="14"/>
-      <c r="R26" s="14"/>
-      <c r="S26" s="14"/>
-      <c r="U26" s="14" t="str">
+      <c r="Q26" s="16"/>
+      <c r="R26" s="16"/>
+      <c r="S26" s="16"/>
+      <c r="U26" s="16" t="str">
         <f>P26</f>
         <v>Return stack</v>
       </c>
-      <c r="V26" s="14"/>
-      <c r="W26" s="14"/>
-      <c r="X26" s="14"/>
-      <c r="Z26" s="14" t="str">
+      <c r="V26" s="16"/>
+      <c r="W26" s="16"/>
+      <c r="X26" s="16"/>
+      <c r="Z26" s="16" t="str">
         <f>U26</f>
         <v>Return stack</v>
       </c>
-      <c r="AA26" s="14"/>
-      <c r="AB26" s="14"/>
-      <c r="AC26" s="14"/>
-      <c r="AE26" s="14" t="str">
+      <c r="AA26" s="16"/>
+      <c r="AB26" s="16"/>
+      <c r="AC26" s="16"/>
+      <c r="AE26" s="16" t="str">
         <f>Z26</f>
         <v>Return stack</v>
       </c>
-      <c r="AF26" s="14"/>
-      <c r="AG26" s="14"/>
-      <c r="AH26" s="14"/>
-      <c r="AJ26" s="14" t="str">
+      <c r="AF26" s="16"/>
+      <c r="AG26" s="16"/>
+      <c r="AH26" s="16"/>
+      <c r="AJ26" s="16" t="str">
         <f>AE26</f>
         <v>Return stack</v>
       </c>
-      <c r="AK26" s="14"/>
-      <c r="AL26" s="14"/>
-      <c r="AM26" s="14"/>
-      <c r="AO26" s="14" t="str">
+      <c r="AK26" s="16"/>
+      <c r="AL26" s="16"/>
+      <c r="AM26" s="16"/>
+      <c r="AO26" s="16" t="str">
         <f>AJ26</f>
         <v>Return stack</v>
       </c>
-      <c r="AP26" s="14"/>
-      <c r="AQ26" s="14"/>
-      <c r="AR26" s="14"/>
-      <c r="AT26" s="14" t="str">
+      <c r="AP26" s="16"/>
+      <c r="AQ26" s="16"/>
+      <c r="AR26" s="16"/>
+      <c r="AT26" s="16" t="str">
         <f>AO26</f>
         <v>Return stack</v>
       </c>
-      <c r="AU26" s="14"/>
-      <c r="AV26" s="14"/>
-      <c r="AW26" s="14"/>
-      <c r="AY26" s="14">
+      <c r="AU26" s="16"/>
+      <c r="AV26" s="16"/>
+      <c r="AW26" s="16"/>
+      <c r="AY26" s="16">
         <f>BD26</f>
         <v>0</v>
       </c>
-      <c r="AZ26" s="14"/>
-      <c r="BA26" s="14"/>
-      <c r="BB26" s="14"/>
-      <c r="BD26" s="14">
+      <c r="AZ26" s="16"/>
+      <c r="BA26" s="16"/>
+      <c r="BB26" s="16"/>
+      <c r="BD26" s="16">
         <f>AU26</f>
         <v>0</v>
       </c>
-      <c r="BE26" s="14"/>
-      <c r="BF26" s="14"/>
-      <c r="BG26" s="14"/>
-      <c r="BI26" s="14">
+      <c r="BE26" s="16"/>
+      <c r="BF26" s="16"/>
+      <c r="BG26" s="16"/>
+      <c r="BI26" s="16">
         <f>BA26</f>
         <v>0</v>
       </c>
-      <c r="BJ26" s="14"/>
-      <c r="BK26" s="14"/>
-      <c r="BL26" s="14"/>
+      <c r="BJ26" s="16"/>
+      <c r="BK26" s="16"/>
+      <c r="BL26" s="16"/>
     </row>
     <row r="27" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
@@ -4002,11 +4002,76 @@
     </row>
   </sheetData>
   <mergeCells count="91">
-    <mergeCell ref="AZ3:BA3"/>
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AZ5:BA5"/>
-    <mergeCell ref="AZ6:BA6"/>
-    <mergeCell ref="AY8:BB8"/>
+    <mergeCell ref="BI16:BL16"/>
+    <mergeCell ref="BI26:BL26"/>
+    <mergeCell ref="BJ3:BK3"/>
+    <mergeCell ref="BJ4:BK4"/>
+    <mergeCell ref="BJ5:BK5"/>
+    <mergeCell ref="BJ6:BK6"/>
+    <mergeCell ref="BI8:BL8"/>
+    <mergeCell ref="AE16:AH16"/>
+    <mergeCell ref="AE26:AH26"/>
+    <mergeCell ref="AF3:AG3"/>
+    <mergeCell ref="AF4:AG4"/>
+    <mergeCell ref="AF5:AG5"/>
+    <mergeCell ref="AF6:AG6"/>
+    <mergeCell ref="AE8:AH8"/>
+    <mergeCell ref="U16:X16"/>
+    <mergeCell ref="U26:X26"/>
+    <mergeCell ref="AA3:AB3"/>
+    <mergeCell ref="AA4:AB4"/>
+    <mergeCell ref="AA5:AB5"/>
+    <mergeCell ref="AA6:AB6"/>
+    <mergeCell ref="Z8:AC8"/>
+    <mergeCell ref="Z16:AC16"/>
+    <mergeCell ref="Z26:AC26"/>
+    <mergeCell ref="V3:W3"/>
+    <mergeCell ref="V4:W4"/>
+    <mergeCell ref="V5:W5"/>
+    <mergeCell ref="V6:W6"/>
+    <mergeCell ref="U8:X8"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="Q4:R4"/>
+    <mergeCell ref="Q5:R5"/>
+    <mergeCell ref="Q6:R6"/>
+    <mergeCell ref="P8:S8"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="F26:I26"/>
+    <mergeCell ref="K26:N26"/>
+    <mergeCell ref="F8:I8"/>
+    <mergeCell ref="K8:N8"/>
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="K16:N16"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="P16:S16"/>
+    <mergeCell ref="P26:S26"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="A16:D16"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="AJ16:AM16"/>
+    <mergeCell ref="AJ26:AM26"/>
+    <mergeCell ref="AP3:AQ3"/>
+    <mergeCell ref="AP4:AQ4"/>
+    <mergeCell ref="AP5:AQ5"/>
+    <mergeCell ref="AP6:AQ6"/>
+    <mergeCell ref="AO8:AR8"/>
+    <mergeCell ref="AO16:AR16"/>
+    <mergeCell ref="AO26:AR26"/>
+    <mergeCell ref="AK3:AL3"/>
+    <mergeCell ref="AK4:AL4"/>
+    <mergeCell ref="AK5:AL5"/>
+    <mergeCell ref="AK6:AL6"/>
+    <mergeCell ref="AJ8:AM8"/>
     <mergeCell ref="BD16:BG16"/>
     <mergeCell ref="BD26:BG26"/>
     <mergeCell ref="AT16:AW16"/>
@@ -4023,76 +4088,11 @@
     <mergeCell ref="BD8:BG8"/>
     <mergeCell ref="AY16:BB16"/>
     <mergeCell ref="AY26:BB26"/>
-    <mergeCell ref="AJ16:AM16"/>
-    <mergeCell ref="AJ26:AM26"/>
-    <mergeCell ref="AP3:AQ3"/>
-    <mergeCell ref="AP4:AQ4"/>
-    <mergeCell ref="AP5:AQ5"/>
-    <mergeCell ref="AP6:AQ6"/>
-    <mergeCell ref="AO8:AR8"/>
-    <mergeCell ref="AO16:AR16"/>
-    <mergeCell ref="AO26:AR26"/>
-    <mergeCell ref="AK3:AL3"/>
-    <mergeCell ref="AK4:AL4"/>
-    <mergeCell ref="AK5:AL5"/>
-    <mergeCell ref="AK6:AL6"/>
-    <mergeCell ref="AJ8:AM8"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="P16:S16"/>
-    <mergeCell ref="P26:S26"/>
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="A16:D16"/>
-    <mergeCell ref="A26:D26"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="F26:I26"/>
-    <mergeCell ref="K26:N26"/>
-    <mergeCell ref="F8:I8"/>
-    <mergeCell ref="K8:N8"/>
-    <mergeCell ref="F16:I16"/>
-    <mergeCell ref="K16:N16"/>
-    <mergeCell ref="L6:M6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="Q4:R4"/>
-    <mergeCell ref="Q5:R5"/>
-    <mergeCell ref="Q6:R6"/>
-    <mergeCell ref="P8:S8"/>
-    <mergeCell ref="U16:X16"/>
-    <mergeCell ref="U26:X26"/>
-    <mergeCell ref="AA3:AB3"/>
-    <mergeCell ref="AA4:AB4"/>
-    <mergeCell ref="AA5:AB5"/>
-    <mergeCell ref="AA6:AB6"/>
-    <mergeCell ref="Z8:AC8"/>
-    <mergeCell ref="Z16:AC16"/>
-    <mergeCell ref="Z26:AC26"/>
-    <mergeCell ref="V3:W3"/>
-    <mergeCell ref="V4:W4"/>
-    <mergeCell ref="V5:W5"/>
-    <mergeCell ref="V6:W6"/>
-    <mergeCell ref="U8:X8"/>
-    <mergeCell ref="AE16:AH16"/>
-    <mergeCell ref="AE26:AH26"/>
-    <mergeCell ref="AF3:AG3"/>
-    <mergeCell ref="AF4:AG4"/>
-    <mergeCell ref="AF5:AG5"/>
-    <mergeCell ref="AF6:AG6"/>
-    <mergeCell ref="AE8:AH8"/>
-    <mergeCell ref="BI16:BL16"/>
-    <mergeCell ref="BI26:BL26"/>
-    <mergeCell ref="BJ3:BK3"/>
-    <mergeCell ref="BJ4:BK4"/>
-    <mergeCell ref="BJ5:BK5"/>
-    <mergeCell ref="BJ6:BK6"/>
-    <mergeCell ref="BI8:BL8"/>
+    <mergeCell ref="AZ3:BA3"/>
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AZ5:BA5"/>
+    <mergeCell ref="AZ6:BA6"/>
+    <mergeCell ref="AY8:BB8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -4159,8 +4159,8 @@
       <c r="H4" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="J4" s="16"/>
-      <c r="K4" s="16"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -4227,7 +4227,7 @@
         <v>60</v>
       </c>
       <c r="J7" s="1" t="str">
-        <f>DEC2HEX(B7,2)</f>
+        <f t="shared" ref="J7:J22" si="6">DEC2HEX(B7,2)</f>
         <v>3C</v>
       </c>
       <c r="K7" s="1"/>
@@ -4241,7 +4241,7 @@
         <v>56</v>
       </c>
       <c r="D8">
-        <f t="shared" ref="D8" si="6">D9+1</f>
+        <f t="shared" ref="D8" si="7">D9+1</f>
         <v>14</v>
       </c>
       <c r="E8">
@@ -4261,7 +4261,7 @@
         <v>56</v>
       </c>
       <c r="J8" s="1" t="str">
-        <f>DEC2HEX(B8,2)</f>
+        <f t="shared" si="6"/>
         <v>38</v>
       </c>
       <c r="K8" s="1"/>
@@ -4275,7 +4275,7 @@
         <v>52</v>
       </c>
       <c r="D9">
-        <f t="shared" ref="D9" si="7">D10+1</f>
+        <f t="shared" ref="D9" si="8">D10+1</f>
         <v>13</v>
       </c>
       <c r="E9">
@@ -4295,7 +4295,7 @@
         <v>52</v>
       </c>
       <c r="J9" s="1" t="str">
-        <f>DEC2HEX(B9,2)</f>
+        <f t="shared" si="6"/>
         <v>34</v>
       </c>
       <c r="K9" s="1"/>
@@ -4309,7 +4309,7 @@
         <v>48</v>
       </c>
       <c r="D10">
-        <f t="shared" ref="D10" si="8">D11+1</f>
+        <f t="shared" ref="D10" si="9">D11+1</f>
         <v>12</v>
       </c>
       <c r="E10">
@@ -4329,7 +4329,7 @@
         <v>48</v>
       </c>
       <c r="J10" s="1" t="str">
-        <f>DEC2HEX(B10,2)</f>
+        <f t="shared" si="6"/>
         <v>30</v>
       </c>
       <c r="K10" s="1"/>
@@ -4343,7 +4343,7 @@
         <v>44</v>
       </c>
       <c r="D11">
-        <f t="shared" ref="D11:D20" si="9">D12+1</f>
+        <f t="shared" ref="D11:D20" si="10">D12+1</f>
         <v>11</v>
       </c>
       <c r="E11">
@@ -4363,7 +4363,7 @@
         <v>44</v>
       </c>
       <c r="J11" s="1" t="str">
-        <f>DEC2HEX(B11,2)</f>
+        <f t="shared" si="6"/>
         <v>2C</v>
       </c>
       <c r="K11" s="1"/>
@@ -4377,7 +4377,7 @@
         <v>40</v>
       </c>
       <c r="D12">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>10</v>
       </c>
       <c r="E12">
@@ -4397,7 +4397,7 @@
         <v>40</v>
       </c>
       <c r="J12" s="1" t="str">
-        <f>DEC2HEX(B12,2)</f>
+        <f t="shared" si="6"/>
         <v>28</v>
       </c>
       <c r="K12" s="1"/>
@@ -4411,7 +4411,7 @@
         <v>36</v>
       </c>
       <c r="D13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>9</v>
       </c>
       <c r="E13">
@@ -4431,7 +4431,7 @@
         <v>36</v>
       </c>
       <c r="J13" s="1" t="str">
-        <f>DEC2HEX(B13,2)</f>
+        <f t="shared" si="6"/>
         <v>24</v>
       </c>
       <c r="K13" s="1"/>
@@ -4445,7 +4445,7 @@
         <v>32</v>
       </c>
       <c r="D14">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>8</v>
       </c>
       <c r="E14">
@@ -4465,7 +4465,7 @@
         <v>32</v>
       </c>
       <c r="J14" s="1" t="str">
-        <f>DEC2HEX(B14,2)</f>
+        <f t="shared" si="6"/>
         <v>20</v>
       </c>
       <c r="K14" s="1"/>
@@ -4479,7 +4479,7 @@
         <v>28</v>
       </c>
       <c r="D15">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>7</v>
       </c>
       <c r="E15">
@@ -4499,7 +4499,7 @@
         <v>28</v>
       </c>
       <c r="J15" s="1" t="str">
-        <f>DEC2HEX(B15,2)</f>
+        <f t="shared" si="6"/>
         <v>1C</v>
       </c>
       <c r="K15" s="1"/>
@@ -4513,7 +4513,7 @@
         <v>24</v>
       </c>
       <c r="D16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>6</v>
       </c>
       <c r="E16">
@@ -4533,7 +4533,7 @@
         <v>24</v>
       </c>
       <c r="J16" s="1" t="str">
-        <f>DEC2HEX(B16,2)</f>
+        <f t="shared" si="6"/>
         <v>18</v>
       </c>
       <c r="K16" s="1"/>
@@ -4547,7 +4547,7 @@
         <v>20</v>
       </c>
       <c r="D17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5</v>
       </c>
       <c r="E17">
@@ -4567,7 +4567,7 @@
         <v>20</v>
       </c>
       <c r="J17" s="1" t="str">
-        <f>DEC2HEX(B17,2)</f>
+        <f t="shared" si="6"/>
         <v>14</v>
       </c>
       <c r="K17" s="1"/>
@@ -4581,7 +4581,7 @@
         <v>16</v>
       </c>
       <c r="D18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>4</v>
       </c>
       <c r="E18">
@@ -4601,7 +4601,7 @@
         <v>16</v>
       </c>
       <c r="J18" s="1" t="str">
-        <f>DEC2HEX(B18,2)</f>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="K18" s="1"/>
@@ -4615,7 +4615,7 @@
         <v>12</v>
       </c>
       <c r="D19">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>3</v>
       </c>
       <c r="E19">
@@ -4635,7 +4635,7 @@
         <v>12</v>
       </c>
       <c r="J19" s="1" t="str">
-        <f>DEC2HEX(B19,2)</f>
+        <f t="shared" si="6"/>
         <v>0C</v>
       </c>
       <c r="K19" s="1"/>
@@ -4649,7 +4649,7 @@
         <v>8</v>
       </c>
       <c r="D20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
       <c r="E20">
@@ -4669,7 +4669,7 @@
         <v>8</v>
       </c>
       <c r="J20" s="1" t="str">
-        <f>DEC2HEX(B20,2)</f>
+        <f t="shared" si="6"/>
         <v>08</v>
       </c>
       <c r="K20" s="1"/>
@@ -4703,7 +4703,7 @@
         <v>4</v>
       </c>
       <c r="J21" s="1" t="str">
-        <f>DEC2HEX(B21,2)</f>
+        <f t="shared" si="6"/>
         <v>04</v>
       </c>
       <c r="K21" s="1"/>
@@ -4732,7 +4732,7 @@
         <v>0</v>
       </c>
       <c r="J22" s="1" t="str">
-        <f>DEC2HEX(B22,2)</f>
+        <f t="shared" si="6"/>
         <v>00</v>
       </c>
       <c r="K22" s="1"/>
@@ -4746,8 +4746,8 @@
         <v>2</v>
       </c>
       <c r="B24" s="2"/>
-      <c r="J24" s="16"/>
-      <c r="K24" s="16"/>
+      <c r="J24" s="14"/>
+      <c r="K24" s="14"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
@@ -4792,7 +4792,7 @@
         <v>271</v>
       </c>
       <c r="F27">
-        <f t="shared" ref="F27" si="10">E28+1</f>
+        <f t="shared" ref="F27" si="11">E28+1</f>
         <v>256</v>
       </c>
       <c r="H27">
@@ -4807,31 +4807,31 @@
         <v>15</v>
       </c>
       <c r="B28">
-        <f t="shared" ref="B28:B33" si="11">B29+4</f>
+        <f t="shared" ref="B28:B33" si="12">B29+4</f>
         <v>156</v>
       </c>
       <c r="D28">
-        <f t="shared" ref="D28:D33" si="12">D29+1</f>
+        <f t="shared" ref="D28:D33" si="13">D29+1</f>
         <v>7</v>
       </c>
       <c r="E28">
-        <f t="shared" ref="E28:E34" si="13">F28+32-1</f>
+        <f t="shared" ref="E28:E34" si="14">F28+32-1</f>
         <v>255</v>
       </c>
       <c r="F28">
-        <f t="shared" ref="F28:F33" si="14">E29+1</f>
+        <f t="shared" ref="F28:F33" si="15">E29+1</f>
         <v>224</v>
       </c>
       <c r="G28">
-        <f t="shared" ref="G28:G33" si="15">H28+3</f>
+        <f t="shared" ref="G28:G33" si="16">H28+3</f>
         <v>31</v>
       </c>
       <c r="H28">
-        <f t="shared" ref="H28:H33" si="16">G29+1</f>
+        <f t="shared" ref="H28:H33" si="17">G29+1</f>
         <v>28</v>
       </c>
       <c r="J28" s="1" t="str">
-        <f>DEC2HEX(B28,2)</f>
+        <f t="shared" ref="J28:J35" si="18">DEC2HEX(B28,2)</f>
         <v>9C</v>
       </c>
       <c r="K28" s="1"/>
@@ -4841,31 +4841,31 @@
         <v>15</v>
       </c>
       <c r="B29">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>152</v>
       </c>
       <c r="D29">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>6</v>
       </c>
       <c r="E29">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>223</v>
       </c>
       <c r="F29">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>192</v>
       </c>
       <c r="G29">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>27</v>
       </c>
       <c r="H29">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>24</v>
       </c>
       <c r="J29" s="1" t="str">
-        <f>DEC2HEX(B29,2)</f>
+        <f t="shared" si="18"/>
         <v>98</v>
       </c>
       <c r="K29" s="1"/>
@@ -4875,31 +4875,31 @@
         <v>15</v>
       </c>
       <c r="B30">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>148</v>
       </c>
       <c r="D30">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>5</v>
       </c>
       <c r="E30">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>191</v>
       </c>
       <c r="F30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>160</v>
       </c>
       <c r="G30">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>23</v>
       </c>
       <c r="H30">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>20</v>
       </c>
       <c r="J30" s="1" t="str">
-        <f>DEC2HEX(B30,2)</f>
+        <f t="shared" si="18"/>
         <v>94</v>
       </c>
       <c r="K30" s="1"/>
@@ -4909,31 +4909,31 @@
         <v>53</v>
       </c>
       <c r="B31">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>144</v>
       </c>
       <c r="D31">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>4</v>
       </c>
       <c r="E31">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>159</v>
       </c>
       <c r="F31">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>128</v>
       </c>
       <c r="G31">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>19</v>
       </c>
       <c r="H31">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>16</v>
       </c>
       <c r="J31" s="1" t="str">
-        <f>DEC2HEX(B31,2)</f>
+        <f t="shared" si="18"/>
         <v>90</v>
       </c>
       <c r="K31" s="1"/>
@@ -4943,31 +4943,31 @@
         <v>52</v>
       </c>
       <c r="B32">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>140</v>
       </c>
       <c r="D32">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>3</v>
       </c>
       <c r="E32">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>127</v>
       </c>
       <c r="F32">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>96</v>
       </c>
       <c r="G32">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>15</v>
       </c>
       <c r="H32">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>12</v>
       </c>
       <c r="J32" s="1" t="str">
-        <f>DEC2HEX(B32,2)</f>
+        <f t="shared" si="18"/>
         <v>8C</v>
       </c>
       <c r="K32" s="1"/>
@@ -4977,31 +4977,31 @@
         <v>51</v>
       </c>
       <c r="B33">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>136</v>
       </c>
       <c r="D33">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>2</v>
       </c>
       <c r="E33">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>95</v>
       </c>
       <c r="F33">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>64</v>
       </c>
       <c r="G33">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>11</v>
       </c>
       <c r="H33">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>8</v>
       </c>
       <c r="J33" s="1" t="str">
-        <f>DEC2HEX(B33,2)</f>
+        <f t="shared" si="18"/>
         <v>88</v>
       </c>
       <c r="K33" s="1"/>
@@ -5019,7 +5019,7 @@
         <v>1</v>
       </c>
       <c r="E34">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>63</v>
       </c>
       <c r="F34">
@@ -5035,7 +5035,7 @@
         <v>4</v>
       </c>
       <c r="J34" s="1" t="str">
-        <f>DEC2HEX(B34,2)</f>
+        <f t="shared" si="18"/>
         <v>84</v>
       </c>
       <c r="K34" s="1"/>
@@ -5064,7 +5064,7 @@
         <v>0</v>
       </c>
       <c r="J35" s="1" t="str">
-        <f>DEC2HEX(B35,2)</f>
+        <f t="shared" si="18"/>
         <v>80</v>
       </c>
       <c r="K35" s="1"/>

</xml_diff>

<commit_message>
Reduced with of subroutine stack to 10 locals from 16, thus freeing 24 RAM BLOCKS
</commit_message>
<xml_diff>
--- a/Resources/Stack diagrams.xlsx
+++ b/Resources/Stack diagrams.xlsx
@@ -235,7 +235,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -263,6 +263,13 @@
       <color theme="1"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -297,7 +304,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -333,11 +340,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -661,15 +672,15 @@
     </row>
     <row r="3" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
       <c r="D3" s="7"/>
       <c r="E3" s="6"/>
       <c r="F3" s="7"/>
-      <c r="G3" s="15" t="s">
+      <c r="G3" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="15"/>
+      <c r="H3" s="16"/>
       <c r="I3" s="7" t="s">
         <v>60</v>
       </c>
@@ -677,280 +688,280 @@
       <c r="K3" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="L3" s="15" t="s">
+      <c r="L3" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="M3" s="15"/>
+      <c r="M3" s="16"/>
       <c r="N3" s="7">
         <v>14</v>
       </c>
       <c r="P3" s="7"/>
-      <c r="Q3" s="15" t="s">
+      <c r="Q3" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="R3" s="15"/>
+      <c r="R3" s="16"/>
       <c r="S3" s="7">
         <v>41</v>
       </c>
       <c r="U3" s="7"/>
-      <c r="V3" s="15" t="s">
+      <c r="V3" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="W3" s="15"/>
+      <c r="W3" s="16"/>
       <c r="X3" s="7"/>
       <c r="Z3" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="AA3" s="15" t="s">
+      <c r="AA3" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="AB3" s="15"/>
+      <c r="AB3" s="16"/>
       <c r="AC3" s="7" t="s">
         <v>63</v>
       </c>
       <c r="AE3" s="7"/>
-      <c r="AF3" s="15" t="s">
+      <c r="AF3" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="AG3" s="15"/>
+      <c r="AG3" s="16"/>
       <c r="AH3" s="7"/>
       <c r="AJ3" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="AK3" s="15" t="s">
+      <c r="AK3" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="AL3" s="15"/>
+      <c r="AL3" s="16"/>
       <c r="AM3" s="7">
         <v>23</v>
       </c>
       <c r="AO3" s="7"/>
-      <c r="AP3" s="15" t="s">
+      <c r="AP3" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="AQ3" s="15"/>
+      <c r="AQ3" s="16"/>
       <c r="AR3" s="7" t="s">
         <v>65</v>
       </c>
       <c r="AT3" s="7"/>
-      <c r="AU3" s="15" t="s">
+      <c r="AU3" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="AV3" s="15"/>
+      <c r="AV3" s="16"/>
       <c r="AW3" s="7"/>
       <c r="AY3" s="7"/>
-      <c r="AZ3" s="15" t="s">
+      <c r="AZ3" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="BA3" s="15"/>
+      <c r="BA3" s="16"/>
       <c r="BB3" s="7"/>
       <c r="BD3" s="7"/>
-      <c r="BE3" s="15" t="s">
+      <c r="BE3" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="BF3" s="15"/>
+      <c r="BF3" s="16"/>
       <c r="BG3" s="7">
         <v>0</v>
       </c>
       <c r="BI3" s="7"/>
-      <c r="BJ3" s="15" t="s">
+      <c r="BJ3" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="BK3" s="15"/>
+      <c r="BK3" s="16"/>
       <c r="BL3" s="7"/>
     </row>
     <row r="4" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
       <c r="D4" s="7"/>
       <c r="E4" s="6"/>
       <c r="F4" s="7"/>
-      <c r="G4" s="15" t="s">
+      <c r="G4" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="15"/>
+      <c r="H4" s="16"/>
       <c r="I4" s="7"/>
       <c r="J4" s="6"/>
       <c r="K4" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="L4" s="15"/>
-      <c r="M4" s="15"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="16"/>
       <c r="N4" s="7"/>
       <c r="P4" s="7"/>
-      <c r="Q4" s="15" t="s">
+      <c r="Q4" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="R4" s="15"/>
+      <c r="R4" s="16"/>
       <c r="S4" s="7"/>
       <c r="U4" s="7"/>
-      <c r="V4" s="15"/>
-      <c r="W4" s="15"/>
+      <c r="V4" s="16"/>
+      <c r="W4" s="16"/>
       <c r="X4" s="7"/>
       <c r="Z4" s="7">
         <v>12</v>
       </c>
-      <c r="AA4" s="15"/>
-      <c r="AB4" s="15"/>
+      <c r="AA4" s="16"/>
+      <c r="AB4" s="16"/>
       <c r="AC4" s="7"/>
       <c r="AE4" s="7"/>
-      <c r="AF4" s="15"/>
-      <c r="AG4" s="15"/>
+      <c r="AF4" s="16"/>
+      <c r="AG4" s="16"/>
       <c r="AH4" s="7"/>
       <c r="AJ4" s="7">
         <v>20</v>
       </c>
-      <c r="AK4" s="15"/>
-      <c r="AL4" s="15"/>
+      <c r="AK4" s="16"/>
+      <c r="AL4" s="16"/>
       <c r="AM4" s="7"/>
       <c r="AO4" s="7">
         <v>28</v>
       </c>
-      <c r="AP4" s="15" t="s">
+      <c r="AP4" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="AQ4" s="15"/>
+      <c r="AQ4" s="16"/>
       <c r="AR4" s="7"/>
       <c r="AT4" s="7"/>
-      <c r="AU4" s="15"/>
-      <c r="AV4" s="15"/>
+      <c r="AU4" s="16"/>
+      <c r="AV4" s="16"/>
       <c r="AW4" s="7"/>
       <c r="AY4" s="7"/>
-      <c r="AZ4" s="15"/>
-      <c r="BA4" s="15"/>
+      <c r="AZ4" s="16"/>
+      <c r="BA4" s="16"/>
       <c r="BB4" s="7"/>
       <c r="BD4" s="7"/>
-      <c r="BE4" s="15" t="s">
+      <c r="BE4" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="BF4" s="15"/>
+      <c r="BF4" s="16"/>
       <c r="BG4" s="7"/>
       <c r="BI4" s="7"/>
-      <c r="BJ4" s="15"/>
-      <c r="BK4" s="15"/>
+      <c r="BJ4" s="16"/>
+      <c r="BK4" s="16"/>
       <c r="BL4" s="7"/>
     </row>
     <row r="5" spans="1:64" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
       <c r="D5" s="7"/>
       <c r="E5" s="6"/>
       <c r="F5" s="7"/>
-      <c r="G5" s="15" t="s">
+      <c r="G5" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="15"/>
+      <c r="H5" s="16"/>
       <c r="I5" s="7" t="s">
         <v>59</v>
       </c>
       <c r="J5" s="6"/>
       <c r="K5" s="7"/>
-      <c r="L5" s="15"/>
-      <c r="M5" s="15"/>
+      <c r="L5" s="16"/>
+      <c r="M5" s="16"/>
       <c r="N5" s="7"/>
       <c r="P5" s="7"/>
-      <c r="Q5" s="15"/>
-      <c r="R5" s="15"/>
+      <c r="Q5" s="16"/>
+      <c r="R5" s="16"/>
       <c r="S5" s="7"/>
       <c r="U5" s="7"/>
-      <c r="V5" s="15"/>
-      <c r="W5" s="15"/>
+      <c r="V5" s="16"/>
+      <c r="W5" s="16"/>
       <c r="X5" s="7"/>
       <c r="Z5" s="7"/>
-      <c r="AA5" s="15"/>
-      <c r="AB5" s="15"/>
+      <c r="AA5" s="16"/>
+      <c r="AB5" s="16"/>
       <c r="AC5" s="7"/>
       <c r="AE5" s="7"/>
-      <c r="AF5" s="15"/>
-      <c r="AG5" s="15"/>
+      <c r="AF5" s="16"/>
+      <c r="AG5" s="16"/>
       <c r="AH5" s="7"/>
       <c r="AJ5" s="7"/>
-      <c r="AK5" s="15"/>
-      <c r="AL5" s="15"/>
+      <c r="AK5" s="16"/>
+      <c r="AL5" s="16"/>
       <c r="AM5" s="7"/>
       <c r="AO5" s="7">
         <v>29</v>
       </c>
-      <c r="AP5" s="15" t="s">
+      <c r="AP5" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="AQ5" s="15"/>
+      <c r="AQ5" s="16"/>
       <c r="AR5" s="7"/>
       <c r="AT5" s="7"/>
-      <c r="AU5" s="15"/>
-      <c r="AV5" s="15"/>
+      <c r="AU5" s="16"/>
+      <c r="AV5" s="16"/>
       <c r="AW5" s="7"/>
       <c r="AY5" s="7"/>
-      <c r="AZ5" s="15"/>
-      <c r="BA5" s="15"/>
+      <c r="AZ5" s="16"/>
+      <c r="BA5" s="16"/>
       <c r="BB5" s="7"/>
       <c r="BD5" s="7"/>
-      <c r="BE5" s="15"/>
-      <c r="BF5" s="15"/>
+      <c r="BE5" s="16"/>
+      <c r="BF5" s="16"/>
       <c r="BG5" s="7"/>
       <c r="BI5" s="7"/>
-      <c r="BJ5" s="15"/>
-      <c r="BK5" s="15"/>
+      <c r="BJ5" s="16"/>
+      <c r="BK5" s="16"/>
       <c r="BL5" s="7"/>
     </row>
     <row r="6" spans="1:64" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="7"/>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="16"/>
       <c r="D6" s="7"/>
       <c r="F6" s="7"/>
-      <c r="G6" s="15" t="s">
+      <c r="G6" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="15"/>
+      <c r="H6" s="16"/>
       <c r="I6" s="7"/>
       <c r="K6" s="7"/>
-      <c r="L6" s="15"/>
-      <c r="M6" s="15"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="16"/>
       <c r="N6" s="7"/>
       <c r="P6" s="7"/>
-      <c r="Q6" s="15"/>
-      <c r="R6" s="15"/>
+      <c r="Q6" s="16"/>
+      <c r="R6" s="16"/>
       <c r="S6" s="7"/>
       <c r="U6" s="7"/>
-      <c r="V6" s="15"/>
-      <c r="W6" s="15"/>
+      <c r="V6" s="16"/>
+      <c r="W6" s="16"/>
       <c r="X6" s="7"/>
       <c r="Z6" s="7"/>
-      <c r="AA6" s="15"/>
-      <c r="AB6" s="15"/>
+      <c r="AA6" s="16"/>
+      <c r="AB6" s="16"/>
       <c r="AC6" s="7"/>
       <c r="AE6" s="7"/>
-      <c r="AF6" s="15"/>
-      <c r="AG6" s="15"/>
+      <c r="AF6" s="16"/>
+      <c r="AG6" s="16"/>
       <c r="AH6" s="7"/>
       <c r="AJ6" s="7"/>
-      <c r="AK6" s="15"/>
-      <c r="AL6" s="15"/>
+      <c r="AK6" s="16"/>
+      <c r="AL6" s="16"/>
       <c r="AM6" s="7"/>
       <c r="AO6" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="AP6" s="15"/>
-      <c r="AQ6" s="15"/>
+      <c r="AP6" s="16"/>
+      <c r="AQ6" s="16"/>
       <c r="AR6" s="7"/>
       <c r="AT6" s="7"/>
-      <c r="AU6" s="15"/>
-      <c r="AV6" s="15"/>
+      <c r="AU6" s="16"/>
+      <c r="AV6" s="16"/>
       <c r="AW6" s="7"/>
       <c r="AY6" s="7"/>
-      <c r="AZ6" s="15"/>
-      <c r="BA6" s="15"/>
+      <c r="AZ6" s="16"/>
+      <c r="BA6" s="16"/>
       <c r="BB6" s="7"/>
       <c r="BD6" s="7"/>
-      <c r="BE6" s="15"/>
-      <c r="BF6" s="15"/>
+      <c r="BE6" s="16"/>
+      <c r="BF6" s="16"/>
       <c r="BG6" s="7"/>
       <c r="BI6" s="7"/>
-      <c r="BJ6" s="15"/>
-      <c r="BK6" s="15"/>
+      <c r="BJ6" s="16"/>
+      <c r="BK6" s="16"/>
       <c r="BL6" s="7"/>
     </row>
     <row r="7" spans="1:64" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1008,84 +1019,84 @@
       <c r="BL7" s="13"/>
     </row>
     <row r="8" spans="1:64" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="F8" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="16"/>
-      <c r="K8" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="L8" s="16"/>
-      <c r="M8" s="16"/>
-      <c r="N8" s="16"/>
-      <c r="P8" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q8" s="16"/>
-      <c r="R8" s="16"/>
-      <c r="S8" s="16"/>
-      <c r="U8" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="V8" s="16"/>
-      <c r="W8" s="16"/>
-      <c r="X8" s="16"/>
-      <c r="Z8" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="AA8" s="16"/>
-      <c r="AB8" s="16"/>
-      <c r="AC8" s="16"/>
-      <c r="AE8" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="AF8" s="16"/>
-      <c r="AG8" s="16"/>
-      <c r="AH8" s="16"/>
-      <c r="AJ8" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="AK8" s="16"/>
-      <c r="AL8" s="16"/>
-      <c r="AM8" s="16"/>
-      <c r="AO8" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="AP8" s="16"/>
-      <c r="AQ8" s="16"/>
-      <c r="AR8" s="16"/>
-      <c r="AT8" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="AU8" s="16"/>
-      <c r="AV8" s="16"/>
-      <c r="AW8" s="16"/>
-      <c r="AY8" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="AZ8" s="16"/>
-      <c r="BA8" s="16"/>
-      <c r="BB8" s="16"/>
-      <c r="BD8" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="BE8" s="16"/>
-      <c r="BF8" s="16"/>
-      <c r="BG8" s="16"/>
-      <c r="BI8" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="BJ8" s="16"/>
-      <c r="BK8" s="16"/>
-      <c r="BL8" s="16"/>
+      <c r="A8" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="F8" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="K8" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="L8" s="15"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="15"/>
+      <c r="P8" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q8" s="15"/>
+      <c r="R8" s="15"/>
+      <c r="S8" s="15"/>
+      <c r="U8" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="V8" s="15"/>
+      <c r="W8" s="15"/>
+      <c r="X8" s="15"/>
+      <c r="Z8" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA8" s="15"/>
+      <c r="AB8" s="15"/>
+      <c r="AC8" s="15"/>
+      <c r="AE8" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="AF8" s="15"/>
+      <c r="AG8" s="15"/>
+      <c r="AH8" s="15"/>
+      <c r="AJ8" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="AK8" s="15"/>
+      <c r="AL8" s="15"/>
+      <c r="AM8" s="15"/>
+      <c r="AO8" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="AP8" s="15"/>
+      <c r="AQ8" s="15"/>
+      <c r="AR8" s="15"/>
+      <c r="AT8" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="AU8" s="15"/>
+      <c r="AV8" s="15"/>
+      <c r="AW8" s="15"/>
+      <c r="AY8" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="AZ8" s="15"/>
+      <c r="BA8" s="15"/>
+      <c r="BB8" s="15"/>
+      <c r="BD8" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="BE8" s="15"/>
+      <c r="BF8" s="15"/>
+      <c r="BG8" s="15"/>
+      <c r="BI8" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="BJ8" s="15"/>
+      <c r="BK8" s="15"/>
+      <c r="BL8" s="15"/>
     </row>
     <row r="9" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -1693,96 +1704,96 @@
       </c>
     </row>
     <row r="16" spans="1:64" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="16" t="s">
+      <c r="A16" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B16" s="16"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="F16" s="16" t="str">
+      <c r="B16" s="15"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="F16" s="15" t="str">
         <f>A16</f>
         <v>Subroutine stack</v>
       </c>
-      <c r="G16" s="16"/>
-      <c r="H16" s="16"/>
-      <c r="I16" s="16"/>
-      <c r="K16" s="16" t="str">
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="15"/>
+      <c r="K16" s="15" t="str">
         <f>F16</f>
         <v>Subroutine stack</v>
       </c>
-      <c r="L16" s="16"/>
-      <c r="M16" s="16"/>
-      <c r="N16" s="16"/>
-      <c r="P16" s="16" t="str">
+      <c r="L16" s="15"/>
+      <c r="M16" s="15"/>
+      <c r="N16" s="15"/>
+      <c r="P16" s="15" t="str">
         <f>K16</f>
         <v>Subroutine stack</v>
       </c>
-      <c r="Q16" s="16"/>
-      <c r="R16" s="16"/>
-      <c r="S16" s="16"/>
-      <c r="U16" s="16" t="str">
+      <c r="Q16" s="15"/>
+      <c r="R16" s="15"/>
+      <c r="S16" s="15"/>
+      <c r="U16" s="15" t="str">
         <f>P16</f>
         <v>Subroutine stack</v>
       </c>
-      <c r="V16" s="16"/>
-      <c r="W16" s="16"/>
-      <c r="X16" s="16"/>
-      <c r="Z16" s="16" t="str">
+      <c r="V16" s="15"/>
+      <c r="W16" s="15"/>
+      <c r="X16" s="15"/>
+      <c r="Z16" s="15" t="str">
         <f>U16</f>
         <v>Subroutine stack</v>
       </c>
-      <c r="AA16" s="16"/>
-      <c r="AB16" s="16"/>
-      <c r="AC16" s="16"/>
-      <c r="AE16" s="16" t="str">
+      <c r="AA16" s="15"/>
+      <c r="AB16" s="15"/>
+      <c r="AC16" s="15"/>
+      <c r="AE16" s="15" t="str">
         <f>Z16</f>
         <v>Subroutine stack</v>
       </c>
-      <c r="AF16" s="16"/>
-      <c r="AG16" s="16"/>
-      <c r="AH16" s="16"/>
-      <c r="AJ16" s="16" t="str">
+      <c r="AF16" s="15"/>
+      <c r="AG16" s="15"/>
+      <c r="AH16" s="15"/>
+      <c r="AJ16" s="15" t="str">
         <f>AE16</f>
         <v>Subroutine stack</v>
       </c>
-      <c r="AK16" s="16"/>
-      <c r="AL16" s="16"/>
-      <c r="AM16" s="16"/>
-      <c r="AO16" s="16" t="str">
+      <c r="AK16" s="15"/>
+      <c r="AL16" s="15"/>
+      <c r="AM16" s="15"/>
+      <c r="AO16" s="15" t="str">
         <f>AJ16</f>
         <v>Subroutine stack</v>
       </c>
-      <c r="AP16" s="16"/>
-      <c r="AQ16" s="16"/>
-      <c r="AR16" s="16"/>
-      <c r="AT16" s="16" t="str">
+      <c r="AP16" s="15"/>
+      <c r="AQ16" s="15"/>
+      <c r="AR16" s="15"/>
+      <c r="AT16" s="15" t="str">
         <f>AO16</f>
         <v>Subroutine stack</v>
       </c>
-      <c r="AU16" s="16"/>
-      <c r="AV16" s="16"/>
-      <c r="AW16" s="16"/>
-      <c r="AY16" s="16">
+      <c r="AU16" s="15"/>
+      <c r="AV16" s="15"/>
+      <c r="AW16" s="15"/>
+      <c r="AY16" s="15">
         <f>BD16</f>
         <v>0</v>
       </c>
-      <c r="AZ16" s="16"/>
-      <c r="BA16" s="16"/>
-      <c r="BB16" s="16"/>
-      <c r="BD16" s="16">
+      <c r="AZ16" s="15"/>
+      <c r="BA16" s="15"/>
+      <c r="BB16" s="15"/>
+      <c r="BD16" s="15">
         <f>AU16</f>
         <v>0</v>
       </c>
-      <c r="BE16" s="16"/>
-      <c r="BF16" s="16"/>
-      <c r="BG16" s="16"/>
-      <c r="BI16" s="16">
+      <c r="BE16" s="15"/>
+      <c r="BF16" s="15"/>
+      <c r="BG16" s="15"/>
+      <c r="BI16" s="15">
         <f>BA16</f>
         <v>0</v>
       </c>
-      <c r="BJ16" s="16"/>
-      <c r="BK16" s="16"/>
-      <c r="BL16" s="16"/>
+      <c r="BJ16" s="15"/>
+      <c r="BK16" s="15"/>
+      <c r="BL16" s="15"/>
     </row>
     <row r="17" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
@@ -2589,96 +2600,96 @@
       </c>
     </row>
     <row r="26" spans="1:64" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="16" t="s">
+      <c r="A26" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B26" s="16"/>
-      <c r="C26" s="16"/>
-      <c r="D26" s="16"/>
-      <c r="F26" s="16" t="str">
+      <c r="B26" s="15"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="15"/>
+      <c r="F26" s="15" t="str">
         <f>A26</f>
         <v>Return stack</v>
       </c>
-      <c r="G26" s="16"/>
-      <c r="H26" s="16"/>
-      <c r="I26" s="16"/>
-      <c r="K26" s="16" t="str">
+      <c r="G26" s="15"/>
+      <c r="H26" s="15"/>
+      <c r="I26" s="15"/>
+      <c r="K26" s="15" t="str">
         <f>F26</f>
         <v>Return stack</v>
       </c>
-      <c r="L26" s="16"/>
-      <c r="M26" s="16"/>
-      <c r="N26" s="16"/>
-      <c r="P26" s="16" t="str">
+      <c r="L26" s="15"/>
+      <c r="M26" s="15"/>
+      <c r="N26" s="15"/>
+      <c r="P26" s="15" t="str">
         <f>K26</f>
         <v>Return stack</v>
       </c>
-      <c r="Q26" s="16"/>
-      <c r="R26" s="16"/>
-      <c r="S26" s="16"/>
-      <c r="U26" s="16" t="str">
+      <c r="Q26" s="15"/>
+      <c r="R26" s="15"/>
+      <c r="S26" s="15"/>
+      <c r="U26" s="15" t="str">
         <f>P26</f>
         <v>Return stack</v>
       </c>
-      <c r="V26" s="16"/>
-      <c r="W26" s="16"/>
-      <c r="X26" s="16"/>
-      <c r="Z26" s="16" t="str">
+      <c r="V26" s="15"/>
+      <c r="W26" s="15"/>
+      <c r="X26" s="15"/>
+      <c r="Z26" s="15" t="str">
         <f>U26</f>
         <v>Return stack</v>
       </c>
-      <c r="AA26" s="16"/>
-      <c r="AB26" s="16"/>
-      <c r="AC26" s="16"/>
-      <c r="AE26" s="16" t="str">
+      <c r="AA26" s="15"/>
+      <c r="AB26" s="15"/>
+      <c r="AC26" s="15"/>
+      <c r="AE26" s="15" t="str">
         <f>Z26</f>
         <v>Return stack</v>
       </c>
-      <c r="AF26" s="16"/>
-      <c r="AG26" s="16"/>
-      <c r="AH26" s="16"/>
-      <c r="AJ26" s="16" t="str">
+      <c r="AF26" s="15"/>
+      <c r="AG26" s="15"/>
+      <c r="AH26" s="15"/>
+      <c r="AJ26" s="15" t="str">
         <f>AE26</f>
         <v>Return stack</v>
       </c>
-      <c r="AK26" s="16"/>
-      <c r="AL26" s="16"/>
-      <c r="AM26" s="16"/>
-      <c r="AO26" s="16" t="str">
+      <c r="AK26" s="15"/>
+      <c r="AL26" s="15"/>
+      <c r="AM26" s="15"/>
+      <c r="AO26" s="15" t="str">
         <f>AJ26</f>
         <v>Return stack</v>
       </c>
-      <c r="AP26" s="16"/>
-      <c r="AQ26" s="16"/>
-      <c r="AR26" s="16"/>
-      <c r="AT26" s="16" t="str">
+      <c r="AP26" s="15"/>
+      <c r="AQ26" s="15"/>
+      <c r="AR26" s="15"/>
+      <c r="AT26" s="15" t="str">
         <f>AO26</f>
         <v>Return stack</v>
       </c>
-      <c r="AU26" s="16"/>
-      <c r="AV26" s="16"/>
-      <c r="AW26" s="16"/>
-      <c r="AY26" s="16">
+      <c r="AU26" s="15"/>
+      <c r="AV26" s="15"/>
+      <c r="AW26" s="15"/>
+      <c r="AY26" s="15">
         <f>BD26</f>
         <v>0</v>
       </c>
-      <c r="AZ26" s="16"/>
-      <c r="BA26" s="16"/>
-      <c r="BB26" s="16"/>
-      <c r="BD26" s="16">
+      <c r="AZ26" s="15"/>
+      <c r="BA26" s="15"/>
+      <c r="BB26" s="15"/>
+      <c r="BD26" s="15">
         <f>AU26</f>
         <v>0</v>
       </c>
-      <c r="BE26" s="16"/>
-      <c r="BF26" s="16"/>
-      <c r="BG26" s="16"/>
-      <c r="BI26" s="16">
+      <c r="BE26" s="15"/>
+      <c r="BF26" s="15"/>
+      <c r="BG26" s="15"/>
+      <c r="BI26" s="15">
         <f>BA26</f>
         <v>0</v>
       </c>
-      <c r="BJ26" s="16"/>
-      <c r="BK26" s="16"/>
-      <c r="BL26" s="16"/>
+      <c r="BJ26" s="15"/>
+      <c r="BK26" s="15"/>
+      <c r="BL26" s="15"/>
     </row>
     <row r="27" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
@@ -4002,76 +4013,11 @@
     </row>
   </sheetData>
   <mergeCells count="91">
-    <mergeCell ref="BI16:BL16"/>
-    <mergeCell ref="BI26:BL26"/>
-    <mergeCell ref="BJ3:BK3"/>
-    <mergeCell ref="BJ4:BK4"/>
-    <mergeCell ref="BJ5:BK5"/>
-    <mergeCell ref="BJ6:BK6"/>
-    <mergeCell ref="BI8:BL8"/>
-    <mergeCell ref="AE16:AH16"/>
-    <mergeCell ref="AE26:AH26"/>
-    <mergeCell ref="AF3:AG3"/>
-    <mergeCell ref="AF4:AG4"/>
-    <mergeCell ref="AF5:AG5"/>
-    <mergeCell ref="AF6:AG6"/>
-    <mergeCell ref="AE8:AH8"/>
-    <mergeCell ref="U16:X16"/>
-    <mergeCell ref="U26:X26"/>
-    <mergeCell ref="AA3:AB3"/>
-    <mergeCell ref="AA4:AB4"/>
-    <mergeCell ref="AA5:AB5"/>
-    <mergeCell ref="AA6:AB6"/>
-    <mergeCell ref="Z8:AC8"/>
-    <mergeCell ref="Z16:AC16"/>
-    <mergeCell ref="Z26:AC26"/>
-    <mergeCell ref="V3:W3"/>
-    <mergeCell ref="V4:W4"/>
-    <mergeCell ref="V5:W5"/>
-    <mergeCell ref="V6:W6"/>
-    <mergeCell ref="U8:X8"/>
-    <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="Q4:R4"/>
-    <mergeCell ref="Q5:R5"/>
-    <mergeCell ref="Q6:R6"/>
-    <mergeCell ref="P8:S8"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="F26:I26"/>
-    <mergeCell ref="K26:N26"/>
-    <mergeCell ref="F8:I8"/>
-    <mergeCell ref="K8:N8"/>
-    <mergeCell ref="F16:I16"/>
-    <mergeCell ref="K16:N16"/>
-    <mergeCell ref="L6:M6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="P16:S16"/>
-    <mergeCell ref="P26:S26"/>
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="A16:D16"/>
-    <mergeCell ref="A26:D26"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="AJ16:AM16"/>
-    <mergeCell ref="AJ26:AM26"/>
-    <mergeCell ref="AP3:AQ3"/>
-    <mergeCell ref="AP4:AQ4"/>
-    <mergeCell ref="AP5:AQ5"/>
-    <mergeCell ref="AP6:AQ6"/>
-    <mergeCell ref="AO8:AR8"/>
-    <mergeCell ref="AO16:AR16"/>
-    <mergeCell ref="AO26:AR26"/>
-    <mergeCell ref="AK3:AL3"/>
-    <mergeCell ref="AK4:AL4"/>
-    <mergeCell ref="AK5:AL5"/>
-    <mergeCell ref="AK6:AL6"/>
-    <mergeCell ref="AJ8:AM8"/>
+    <mergeCell ref="AZ3:BA3"/>
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AZ5:BA5"/>
+    <mergeCell ref="AZ6:BA6"/>
+    <mergeCell ref="AY8:BB8"/>
     <mergeCell ref="BD16:BG16"/>
     <mergeCell ref="BD26:BG26"/>
     <mergeCell ref="AT16:AW16"/>
@@ -4088,11 +4034,76 @@
     <mergeCell ref="BD8:BG8"/>
     <mergeCell ref="AY16:BB16"/>
     <mergeCell ref="AY26:BB26"/>
-    <mergeCell ref="AZ3:BA3"/>
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AZ5:BA5"/>
-    <mergeCell ref="AZ6:BA6"/>
-    <mergeCell ref="AY8:BB8"/>
+    <mergeCell ref="AJ16:AM16"/>
+    <mergeCell ref="AJ26:AM26"/>
+    <mergeCell ref="AP3:AQ3"/>
+    <mergeCell ref="AP4:AQ4"/>
+    <mergeCell ref="AP5:AQ5"/>
+    <mergeCell ref="AP6:AQ6"/>
+    <mergeCell ref="AO8:AR8"/>
+    <mergeCell ref="AO16:AR16"/>
+    <mergeCell ref="AO26:AR26"/>
+    <mergeCell ref="AK3:AL3"/>
+    <mergeCell ref="AK4:AL4"/>
+    <mergeCell ref="AK5:AL5"/>
+    <mergeCell ref="AK6:AL6"/>
+    <mergeCell ref="AJ8:AM8"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="P16:S16"/>
+    <mergeCell ref="P26:S26"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="A16:D16"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="F26:I26"/>
+    <mergeCell ref="K26:N26"/>
+    <mergeCell ref="F8:I8"/>
+    <mergeCell ref="K8:N8"/>
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="K16:N16"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="Q4:R4"/>
+    <mergeCell ref="Q5:R5"/>
+    <mergeCell ref="Q6:R6"/>
+    <mergeCell ref="P8:S8"/>
+    <mergeCell ref="U16:X16"/>
+    <mergeCell ref="U26:X26"/>
+    <mergeCell ref="AA3:AB3"/>
+    <mergeCell ref="AA4:AB4"/>
+    <mergeCell ref="AA5:AB5"/>
+    <mergeCell ref="AA6:AB6"/>
+    <mergeCell ref="Z8:AC8"/>
+    <mergeCell ref="Z16:AC16"/>
+    <mergeCell ref="Z26:AC26"/>
+    <mergeCell ref="V3:W3"/>
+    <mergeCell ref="V4:W4"/>
+    <mergeCell ref="V5:W5"/>
+    <mergeCell ref="V6:W6"/>
+    <mergeCell ref="U8:X8"/>
+    <mergeCell ref="AE16:AH16"/>
+    <mergeCell ref="AE26:AH26"/>
+    <mergeCell ref="AF3:AG3"/>
+    <mergeCell ref="AF4:AG4"/>
+    <mergeCell ref="AF5:AG5"/>
+    <mergeCell ref="AF6:AG6"/>
+    <mergeCell ref="AE8:AH8"/>
+    <mergeCell ref="BI16:BL16"/>
+    <mergeCell ref="BI26:BL26"/>
+    <mergeCell ref="BJ3:BK3"/>
+    <mergeCell ref="BJ4:BK4"/>
+    <mergeCell ref="BJ5:BK5"/>
+    <mergeCell ref="BJ6:BK6"/>
+    <mergeCell ref="BI8:BL8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -4104,7 +4115,7 @@
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:K1048576"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4167,15 +4178,16 @@
         <v>17</v>
       </c>
       <c r="E5">
-        <f>512+31</f>
-        <v>543</v>
+        <f>F6+31</f>
+        <v>351</v>
       </c>
       <c r="F5">
-        <v>535</v>
+        <f>E5-8</f>
+        <v>343</v>
       </c>
       <c r="G5">
         <f>H6+4-1</f>
-        <v>67</v>
+        <v>43</v>
       </c>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
@@ -4185,222 +4197,223 @@
         <v>16</v>
       </c>
       <c r="E6">
-        <v>534</v>
+        <f>F5-1</f>
+        <v>342</v>
       </c>
       <c r="F6">
-        <f>E7+1</f>
-        <v>512</v>
+        <f>E13+1</f>
+        <v>320</v>
       </c>
       <c r="H6">
-        <f>G7+1</f>
-        <v>64</v>
+        <f>G13+1</f>
+        <v>40</v>
       </c>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="17">
         <f t="shared" ref="B7:B20" si="0">B8+4</f>
         <v>60</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="17">
         <f t="shared" ref="D7" si="1">D8+1</f>
         <v>15</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="17">
         <f t="shared" ref="E7:E21" si="2">F7+32-1</f>
         <v>511</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="17">
         <f t="shared" ref="F7:F20" si="3">E8+1</f>
         <v>480</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="17">
         <f t="shared" ref="G7:G20" si="4">H7+3</f>
         <v>63</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="17">
         <f t="shared" ref="H7:H20" si="5">G8+1</f>
         <v>60</v>
       </c>
-      <c r="J7" s="1" t="str">
+      <c r="J7" s="18" t="str">
         <f t="shared" ref="J7:J22" si="6">DEC2HEX(B7,2)</f>
         <v>3C</v>
       </c>
-      <c r="K7" s="1"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="K7" s="18"/>
+    </row>
+    <row r="8" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="17">
         <f t="shared" si="0"/>
         <v>56</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="17">
         <f t="shared" ref="D8" si="7">D9+1</f>
         <v>14</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="17">
         <f t="shared" si="2"/>
         <v>479</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="17">
         <f t="shared" si="3"/>
         <v>448</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="17">
         <f t="shared" si="4"/>
         <v>59</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="17">
         <f t="shared" si="5"/>
         <v>56</v>
       </c>
-      <c r="J8" s="1" t="str">
+      <c r="J8" s="18" t="str">
         <f t="shared" si="6"/>
         <v>38</v>
       </c>
-      <c r="K8" s="1"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="K8" s="18"/>
+    </row>
+    <row r="9" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="17">
         <f t="shared" si="0"/>
         <v>52</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="17">
         <f t="shared" ref="D9" si="8">D10+1</f>
         <v>13</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="17">
         <f t="shared" si="2"/>
         <v>447</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="17">
         <f t="shared" si="3"/>
         <v>416</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="17">
         <f t="shared" si="4"/>
         <v>55</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="17">
         <f t="shared" si="5"/>
         <v>52</v>
       </c>
-      <c r="J9" s="1" t="str">
+      <c r="J9" s="18" t="str">
         <f t="shared" si="6"/>
         <v>34</v>
       </c>
-      <c r="K9" s="1"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="K9" s="18"/>
+    </row>
+    <row r="10" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="17">
         <f t="shared" si="0"/>
         <v>48</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="17">
         <f t="shared" ref="D10" si="9">D11+1</f>
         <v>12</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="17">
         <f t="shared" si="2"/>
         <v>415</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="17">
         <f t="shared" si="3"/>
         <v>384</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="17">
         <f t="shared" si="4"/>
         <v>51</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="17">
         <f t="shared" si="5"/>
         <v>48</v>
       </c>
-      <c r="J10" s="1" t="str">
+      <c r="J10" s="18" t="str">
         <f t="shared" si="6"/>
         <v>30</v>
       </c>
-      <c r="K10" s="1"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="K10" s="18"/>
+    </row>
+    <row r="11" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="17">
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="17">
         <f t="shared" ref="D11:D20" si="10">D12+1</f>
         <v>11</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="17">
         <f t="shared" si="2"/>
         <v>383</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="17">
         <f t="shared" si="3"/>
         <v>352</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="17">
         <f t="shared" si="4"/>
         <v>47</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="17">
         <f t="shared" si="5"/>
         <v>44</v>
       </c>
-      <c r="J11" s="1" t="str">
+      <c r="J11" s="18" t="str">
         <f t="shared" si="6"/>
         <v>2C</v>
       </c>
-      <c r="K11" s="1"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="K11" s="18"/>
+    </row>
+    <row r="12" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="17">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="17">
         <f t="shared" si="10"/>
         <v>10</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="17">
         <f t="shared" si="2"/>
         <v>351</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="17">
         <f t="shared" si="3"/>
         <v>320</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="17">
         <f t="shared" si="4"/>
         <v>43</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="17">
         <f t="shared" si="5"/>
         <v>40</v>
       </c>
-      <c r="J12" s="1" t="str">
+      <c r="J12" s="18" t="str">
         <f t="shared" si="6"/>
         <v>28</v>
       </c>
-      <c r="K12" s="1"/>
+      <c r="K12" s="18"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">

</xml_diff>